<commit_message>
:cat: add incubation for true counts
</commit_message>
<xml_diff>
--- a/data/raw_data/DS_Counting_trials.xlsx
+++ b/data/raw_data/DS_Counting_trials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodenico/Documents/Pro/Articles/2023_LarvCount/Y2023.LarvCount/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C5F9F08-9DA3-C34A-9A61-9BB1B4AED609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F7B9B2-9182-9B49-AF8F-E0F5D07B0ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24560" windowHeight="13380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,17 +19,25 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ObserverCountData!$A$1:$F$601</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1810" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1841" uniqueCount="12">
   <si>
     <t>Sample_ID</t>
   </si>
@@ -386,7 +394,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16028,10 +16036,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9772EB32-8C72-6B4E-B539-09D5516AF006}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16039,252 +16047,345 @@
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31">
         <v>0</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>